<commit_message>
remove duplicate xls versions of 2010 analysis logs, remove unused worksheets from xlsx versions of same
</commit_message>
<xml_diff>
--- a/rhizotron data/2010/analysis log 05-24.xlsx
+++ b/rhizotron data/2010/analysis log 05-24.xlsx
@@ -1,19 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="15200" windowHeight="12020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="114210" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -395,8 +393,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -450,7 +448,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -773,14 +771,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
@@ -3736,43 +3734,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>